<commit_message>
DEF5122 - Click anywhere with coordinate - right and left click with x and y coordinates
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/TestScripts_rightClickTrendsGraph.xlsx
+++ b/NformTester/NformTester/Keywordscripts/TestScripts_rightClickTrendsGraph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16035" windowHeight="12720" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16035" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Scripts" sheetId="4" r:id="rId1"/>
@@ -1378,7 +1378,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8409" uniqueCount="959">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8378" uniqueCount="952">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -4065,23 +4065,7 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Peter</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>NformLogin</t>
-  </si>
-  <si>
-    <t>"Administrator"</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>"admin"</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"localhost"</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Version</t>
@@ -4092,16 +4076,10 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>Create Date</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>;Add Device</t>
-  </si>
-  <si>
     <t>Update Date</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -4159,50 +4137,7 @@
     <t>.NET Framework</t>
   </si>
   <si>
-    <t>Text</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Equal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Current devices: 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Devices</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UPS_10.146.82.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LaunchApplication</t>
-  </si>
-  <si>
-    <t>abc</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CloseApplication</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$Sys_TestObject_NformViewer$</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>;</t>
-  </si>
-  <si>
-    <t>FormInstallationWizard</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D:\\01_project\\NForm\\NForm Test\\Nform_4.9\\ET\\Nform_4.9.2_ET\\CDROM\\Nform_4.9.2_ET.msi</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Apply</t>
@@ -4285,14 +4220,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>T</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>AlarmsGadget</t>
   </si>
   <si>
     <t>CommunicationGadget</t>
+  </si>
+  <si>
+    <t>Kwang</t>
+  </si>
+  <si>
+    <t>C:\\Nform\\bin\\NformViewer.exe</t>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Administrator"</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>"admin"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"localhost"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"RackPDU_126.4.202.215"</t>
+  </si>
+  <si>
+    <t>ContextMenuStrip1</t>
+  </si>
+  <si>
+    <t>CopyData</t>
+  </si>
+  <si>
+    <t>ClickLocation</t>
+  </si>
+  <si>
+    <t>right</t>
   </si>
 </sst>
 </file>
@@ -4303,14 +4271,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -4318,7 +4286,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -4501,7 +4469,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1"/>
     <cellStyle name="常规 2 2" xfId="2"/>
   </cellStyles>
@@ -4526,7 +4494,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4812,20 +4780,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.625" customWidth="1"/>
-    <col min="2" max="2" width="24.375" customWidth="1"/>
-    <col min="5" max="5" width="23.625" customWidth="1"/>
-    <col min="6" max="6" width="27.5" customWidth="1"/>
-    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" ht="25.5">
       <c r="A1" s="1" t="s">
         <v>878</v>
       </c>
@@ -4869,12 +4837,12 @@
         <v>886</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15">
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>887</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>929</v>
+        <v>942</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
@@ -4898,26 +4866,30 @@
         <v>889</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>941</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>943</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>890</v>
       </c>
-      <c r="C3" s="4">
-        <v>2</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>927</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>923</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>926</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>924</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4" t="s">
+        <v>944</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>945</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>946</v>
+      </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
@@ -4925,33 +4897,29 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="2" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
       <c r="C4" s="4">
         <v>3</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>927</v>
+        <v>912</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>891</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4" t="s">
-        <v>892</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>893</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>894</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
@@ -4959,26 +4927,28 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>898</v>
+        <v>893</v>
       </c>
       <c r="B5" s="9">
-        <v>40864</v>
+        <v>41856</v>
       </c>
       <c r="C5" s="4">
         <v>4</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>927</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>874</v>
-      </c>
-      <c r="F5" s="4">
-        <v>4</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+        <v>896</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
@@ -4987,49 +4957,61 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>900</v>
+        <v>894</v>
       </c>
       <c r="B6" s="9">
-        <v>41785</v>
+        <v>41856</v>
       </c>
       <c r="C6" s="4">
         <v>5</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>927</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>925</v>
-      </c>
-      <c r="F6" s="4"/>
+        <v>896</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="G6" s="4" t="s">
-        <v>924</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+        <v>55</v>
+      </c>
+      <c r="H6" s="13">
+        <v>2</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>947</v>
+      </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="6"/>
     </row>
-    <row r="7" spans="1:14" ht="15">
+    <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
-        <v>901</v>
+        <v>895</v>
       </c>
       <c r="B7" s="3">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C7" s="4">
         <v>6</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>899</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="D7" s="7" t="s">
+        <v>896</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="13"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -5039,23 +5021,23 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="4">
         <v>7</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>927</v>
+      <c r="D8" s="7" t="s">
+        <v>896</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>2</v>
+        <v>130</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -5067,22 +5049,22 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="4">
         <v>8</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>927</v>
+      <c r="D9" s="7" t="s">
+        <v>896</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>921</v>
-      </c>
-      <c r="G9" s="11" t="s">
+        <v>948</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>949</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="H9" s="4"/>
@@ -5095,34 +5077,34 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>905</v>
+        <v>899</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>906</v>
+        <v>900</v>
       </c>
       <c r="C10" s="4">
         <v>9</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>927</v>
+        <v>896</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>695</v>
+        <v>19</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>699</v>
+        <v>129</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>7</v>
+        <v>950</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>918</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>919</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>920</v>
+        <v>951</v>
+      </c>
+      <c r="I10" s="11">
+        <v>50</v>
+      </c>
+      <c r="J10" s="11">
+        <v>50</v>
       </c>
       <c r="K10" s="11"/>
       <c r="L10" s="11"/>
@@ -5132,21 +5114,11 @@
     <row r="11" spans="1:14">
       <c r="A11" s="15"/>
       <c r="B11" s="16"/>
-      <c r="C11" s="4">
-        <v>10</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>927</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>695</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>2</v>
-      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
@@ -5157,33 +5129,17 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="2" t="s">
-        <v>907</v>
+        <v>901</v>
       </c>
       <c r="B12" s="17"/>
-      <c r="C12" s="4">
-        <v>11</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>927</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>633</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>918</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>919</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>922</v>
-      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
@@ -5191,21 +5147,13 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="18" t="s">
-        <v>908</v>
+        <v>902</v>
       </c>
       <c r="B13" s="19"/>
-      <c r="C13" s="4">
-        <v>12</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>897</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>874</v>
-      </c>
-      <c r="F13" s="11">
-        <v>40</v>
-      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="13"/>
       <c r="I13" s="11"/>
@@ -5217,24 +5165,14 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="18" t="s">
-        <v>909</v>
+        <v>903</v>
       </c>
       <c r="B14" s="19"/>
-      <c r="C14" s="4">
-        <v>13</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>902</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>928</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>2</v>
-      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
       <c r="J14" s="11"/>
@@ -5245,21 +5183,13 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="18" t="s">
-        <v>910</v>
+        <v>904</v>
       </c>
       <c r="B15" s="19"/>
-      <c r="C15" s="4">
-        <v>14</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>897</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>874</v>
-      </c>
-      <c r="F15" s="11">
-        <v>6</v>
-      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="13"/>
       <c r="I15" s="11"/>
@@ -5271,24 +5201,14 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="18" t="s">
-        <v>911</v>
+        <v>905</v>
       </c>
       <c r="B16" s="19"/>
-      <c r="C16" s="4">
-        <v>15</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>902</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>928</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>791</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>2</v>
-      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
       <c r="H16" s="13"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
@@ -5299,21 +5219,13 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="18" t="s">
-        <v>912</v>
+        <v>906</v>
       </c>
       <c r="B17" s="19"/>
-      <c r="C17" s="4">
-        <v>16</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>897</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>874</v>
-      </c>
-      <c r="F17" s="11">
-        <v>60</v>
-      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="13"/>
       <c r="I17" s="11"/>
@@ -5326,23 +5238,13 @@
     <row r="18" spans="1:14">
       <c r="A18" s="18"/>
       <c r="B18" s="19" t="s">
-        <v>913</v>
-      </c>
-      <c r="C18" s="4">
-        <v>17</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>902</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>928</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>792</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>132</v>
-      </c>
+        <v>907</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
       <c r="J18" s="11"/>
@@ -5354,23 +5256,13 @@
     <row r="19" spans="1:14">
       <c r="A19" s="18"/>
       <c r="B19" s="19" t="s">
-        <v>914</v>
-      </c>
-      <c r="C19" s="4">
-        <v>18</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>902</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>928</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>721</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>2</v>
-      </c>
+        <v>908</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
       <c r="H19" s="13"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
@@ -5381,21 +5273,15 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="18" t="s">
-        <v>915</v>
+        <v>909</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>906</v>
+        <v>900</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="10" t="s">
-        <v>956</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>954</v>
-      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
@@ -5407,7 +5293,7 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="18" t="s">
-        <v>916</v>
+        <v>910</v>
       </c>
       <c r="B21" s="19"/>
       <c r="C21" s="4"/>
@@ -5425,7 +5311,7 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="18" t="s">
-        <v>917</v>
+        <v>911</v>
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="4"/>
@@ -5566,16 +5452,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D6 D8:D30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D4 D10:D30">
       <formula1>"C,F,T,;"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 G4:G5 G7:G30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G9 G11:G30">
       <formula1>INDIRECT(SUBSTITUTE(E2&amp;F2," ",""))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F4:F30">
-      <formula1>OFFSET(INDIRECT($E2),0,0,COUNTA(INDIRECT(E2&amp;"Col")),1)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9 F2:F8 F10:F30">
+      <formula1>OFFSET(INDIRECT($E2),0,0,COUNTA(INDIRECT(D2&amp;"Col")),1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E8 E10:E30">
       <formula1>Forms</formula1>
     </dataValidation>
   </dataValidations>
@@ -5592,11 +5478,11 @@
       <selection activeCell="E131" sqref="E131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.25" customWidth="1"/>
-    <col min="5" max="5" width="35.75" customWidth="1"/>
-    <col min="7" max="7" width="31.25" customWidth="1"/>
+    <col min="1" max="1" width="39.28515625" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:90">
@@ -8744,7 +8630,7 @@
         <v>64</v>
       </c>
       <c r="G38" t="s">
-        <v>930</v>
+        <v>913</v>
       </c>
       <c r="AV38" t="s">
         <v>540</v>
@@ -8764,7 +8650,7 @@
         <v>65</v>
       </c>
       <c r="G39" t="s">
-        <v>931</v>
+        <v>914</v>
       </c>
       <c r="AV39" t="s">
         <v>541</v>
@@ -8784,7 +8670,7 @@
         <v>66</v>
       </c>
       <c r="G40" t="s">
-        <v>932</v>
+        <v>915</v>
       </c>
       <c r="AV40" t="s">
         <v>542</v>
@@ -8804,7 +8690,7 @@
         <v>67</v>
       </c>
       <c r="G41" t="s">
-        <v>933</v>
+        <v>916</v>
       </c>
       <c r="AV41" t="s">
         <v>543</v>
@@ -8824,7 +8710,7 @@
         <v>68</v>
       </c>
       <c r="G42" t="s">
-        <v>934</v>
+        <v>917</v>
       </c>
       <c r="AV42" t="s">
         <v>544</v>
@@ -8844,7 +8730,7 @@
         <v>69</v>
       </c>
       <c r="G43" t="s">
-        <v>935</v>
+        <v>918</v>
       </c>
       <c r="AV43" t="s">
         <v>545</v>
@@ -8864,7 +8750,7 @@
         <v>70</v>
       </c>
       <c r="G44" t="s">
-        <v>936</v>
+        <v>919</v>
       </c>
       <c r="AV44" t="s">
         <v>546</v>
@@ -8884,7 +8770,7 @@
         <v>71</v>
       </c>
       <c r="G45" t="s">
-        <v>937</v>
+        <v>920</v>
       </c>
       <c r="AV45" t="s">
         <v>547</v>
@@ -8904,7 +8790,7 @@
         <v>72</v>
       </c>
       <c r="G46" t="s">
-        <v>938</v>
+        <v>921</v>
       </c>
       <c r="AV46" t="s">
         <v>548</v>
@@ -8924,7 +8810,7 @@
         <v>73</v>
       </c>
       <c r="G47" t="s">
-        <v>939</v>
+        <v>922</v>
       </c>
       <c r="AV47" t="s">
         <v>549</v>
@@ -8944,7 +8830,7 @@
         <v>74</v>
       </c>
       <c r="G48" t="s">
-        <v>940</v>
+        <v>923</v>
       </c>
       <c r="AV48" t="s">
         <v>550</v>
@@ -8964,7 +8850,7 @@
         <v>75</v>
       </c>
       <c r="G49" t="s">
-        <v>941</v>
+        <v>924</v>
       </c>
       <c r="AV49" t="s">
         <v>551</v>
@@ -8984,7 +8870,7 @@
         <v>15</v>
       </c>
       <c r="G50" t="s">
-        <v>942</v>
+        <v>925</v>
       </c>
       <c r="AV50" t="s">
         <v>552</v>
@@ -9004,7 +8890,7 @@
         <v>76</v>
       </c>
       <c r="G51" t="s">
-        <v>943</v>
+        <v>926</v>
       </c>
       <c r="AV51" t="s">
         <v>553</v>
@@ -9024,7 +8910,7 @@
         <v>77</v>
       </c>
       <c r="G52" t="s">
-        <v>944</v>
+        <v>927</v>
       </c>
       <c r="AV52" t="s">
         <v>554</v>
@@ -9044,7 +8930,7 @@
         <v>78</v>
       </c>
       <c r="G53" t="s">
-        <v>945</v>
+        <v>928</v>
       </c>
       <c r="AV53" t="s">
         <v>555</v>
@@ -9064,7 +8950,7 @@
         <v>79</v>
       </c>
       <c r="G54" t="s">
-        <v>946</v>
+        <v>929</v>
       </c>
       <c r="AV54" t="s">
         <v>556</v>
@@ -9084,7 +8970,7 @@
         <v>80</v>
       </c>
       <c r="G55" t="s">
-        <v>947</v>
+        <v>930</v>
       </c>
       <c r="AV55" t="s">
         <v>557</v>
@@ -9104,7 +8990,7 @@
         <v>81</v>
       </c>
       <c r="G56" t="s">
-        <v>948</v>
+        <v>931</v>
       </c>
       <c r="AV56" t="s">
         <v>558</v>
@@ -9121,7 +9007,7 @@
         <v>82</v>
       </c>
       <c r="G57" t="s">
-        <v>949</v>
+        <v>932</v>
       </c>
       <c r="AV57" t="s">
         <v>559</v>
@@ -9138,7 +9024,7 @@
         <v>83</v>
       </c>
       <c r="G58" t="s">
-        <v>950</v>
+        <v>933</v>
       </c>
       <c r="AV58" t="s">
         <v>560</v>
@@ -9155,7 +9041,7 @@
         <v>84</v>
       </c>
       <c r="G59" t="s">
-        <v>951</v>
+        <v>934</v>
       </c>
       <c r="AV59" t="s">
         <v>561</v>
@@ -9172,7 +9058,7 @@
         <v>85</v>
       </c>
       <c r="G60" t="s">
-        <v>952</v>
+        <v>935</v>
       </c>
       <c r="AV60" t="s">
         <v>562</v>
@@ -9189,7 +9075,7 @@
         <v>86</v>
       </c>
       <c r="G61" t="s">
-        <v>953</v>
+        <v>936</v>
       </c>
       <c r="AV61" t="s">
         <v>563</v>
@@ -9203,7 +9089,7 @@
         <v>87</v>
       </c>
       <c r="G62" t="s">
-        <v>954</v>
+        <v>937</v>
       </c>
       <c r="AV62" t="s">
         <v>564</v>
@@ -9837,7 +9723,7 @@
     </row>
     <row r="130" spans="5:48">
       <c r="E130" t="s">
-        <v>957</v>
+        <v>939</v>
       </c>
       <c r="AV130" t="s">
         <v>626</v>
@@ -9845,7 +9731,7 @@
     </row>
     <row r="131" spans="5:48">
       <c r="E131" t="s">
-        <v>958</v>
+        <v>940</v>
       </c>
     </row>
   </sheetData>
@@ -9858,11 +9744,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:ASE12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CS1" workbookViewId="0">
-      <selection activeCell="CV10" sqref="CV10"/>
+    <sheetView topLeftCell="CS1" workbookViewId="0">
+      <selection activeCell="DB12" sqref="DB12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1175">
       <c r="A1" t="s">
@@ -29090,7 +28976,7 @@
         <v>8</v>
       </c>
       <c r="GW7" t="s">
-        <v>955</v>
+        <v>938</v>
       </c>
       <c r="GZ7" t="s">
         <v>8</v>

</xml_diff>